<commit_message>
closed `240113piu_a` test PASS
</commit_message>
<xml_diff>
--- a/xl2roefact/excel_invoice_template/invoice_template_CU_tva.xlsx
+++ b/xl2roefact/excel_invoice_template/invoice_template_CU_tva.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <r>
       <rPr>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t xml:space="preserve">----adresa.client----</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tara:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RO</t>
   </si>
   <si>
     <t xml:space="preserve">Email:</t>
@@ -925,7 +931,7 @@
   <dimension ref="A2:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.4140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1114,41 +1120,40 @@
       <c r="AMJ12" s="0"/>
     </row>
     <row r="13" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
+      <c r="F13" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
       <c r="AMF13" s="0"/>
       <c r="AMG13" s="0"/>
       <c r="AMH13" s="0"/>
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
-    <row r="14" s="30" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="31" t="s">
+    <row r="14" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="24" t="s">
         <v>26</v>
-      </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>27</v>
       </c>
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
@@ -1161,17 +1166,17 @@
     </row>
     <row r="15" s="30" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="32" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>29</v>
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
@@ -1182,19 +1187,19 @@
       <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
     </row>
-    <row r="16" s="30" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" s="30" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="D16" s="29"/>
+      <c r="E16" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="24" t="s">
         <v>32</v>
-      </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>33</v>
       </c>
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
@@ -1205,89 +1210,83 @@
       <c r="AMI16" s="0"/>
       <c r="AMJ16" s="0"/>
     </row>
-    <row r="17" s="30" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="35"/>
+    <row r="17" s="30" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B17" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>34</v>
+      </c>
       <c r="D17" s="34"/>
+      <c r="E17" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
       <c r="AMF17" s="0"/>
       <c r="AMG17" s="0"/>
       <c r="AMH17" s="0"/>
       <c r="AMI17" s="0"/>
       <c r="AMJ17" s="0"/>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-    </row>
-    <row r="19" s="43" customFormat="true" ht="23.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="38" t="s">
+    <row r="18" s="30" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="35"/>
+      <c r="D18" s="34"/>
+      <c r="AMF18" s="0"/>
+      <c r="AMG18" s="0"/>
+      <c r="AMH18" s="0"/>
+      <c r="AMI18" s="0"/>
+      <c r="AMJ18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+    </row>
+    <row r="20" s="43" customFormat="true" ht="23.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="B20" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="41" t="s">
+      <c r="C20" s="39"/>
+      <c r="D20" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="42" t="s">
+      <c r="E20" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="42" t="s">
+      <c r="F20" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="I19" s="42" t="s">
+      <c r="G20" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="AMF19" s="44"/>
-      <c r="AMG19" s="44"/>
-      <c r="AMH19" s="44"/>
-      <c r="AMI19" s="44"/>
-      <c r="AMJ19" s="44"/>
-    </row>
-    <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="B20" s="46" t="s">
+      <c r="H20" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="45" t="s">
+      <c r="I20" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="F20" s="48" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G20" s="49" t="n">
-        <f aca="false">ROUND(E20*F20,2)</f>
-        <v>1000</v>
-      </c>
-      <c r="H20" s="50" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="I20" s="49" t="n">
-        <f aca="false">ROUND(G20*H20,2)</f>
-        <v>190</v>
-      </c>
+      <c r="AMF20" s="44"/>
+      <c r="AMG20" s="44"/>
+      <c r="AMH20" s="44"/>
+      <c r="AMI20" s="44"/>
+      <c r="AMJ20" s="44"/>
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" s="46" t="s">
         <v>44</v>
@@ -1297,31 +1296,49 @@
         <v>45</v>
       </c>
       <c r="E21" s="47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" s="48" t="n">
-        <v>550</v>
+        <v>1000</v>
       </c>
       <c r="G21" s="49" t="n">
         <f aca="false">ROUND(E21*F21,2)</f>
-        <v>1100</v>
-      </c>
-      <c r="H21" s="50"/>
+        <v>1000</v>
+      </c>
+      <c r="H21" s="50" t="n">
+        <v>0.19</v>
+      </c>
       <c r="I21" s="49" t="n">
         <f aca="false">ROUND(G21*H21,2)</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="45" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="46"/>
+      <c r="D22" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" s="48" t="n">
+        <v>550</v>
+      </c>
+      <c r="G22" s="49" t="n">
+        <f aca="false">ROUND(E22*F22,2)</f>
+        <v>1100</v>
+      </c>
+      <c r="H22" s="50"/>
+      <c r="I22" s="49" t="n">
+        <f aca="false">ROUND(G22*H22,2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="45"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="49"/>
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="45"/>
@@ -1336,8 +1353,8 @@
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="45"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="45"/>
       <c r="E24" s="47"/>
       <c r="F24" s="48"/>
@@ -1367,42 +1384,27 @@
       <c r="H26" s="50"/>
       <c r="I26" s="49"/>
     </row>
-    <row r="27" s="56" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="52"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="AMF27" s="0"/>
-      <c r="AMG27" s="0"/>
-      <c r="AMH27" s="0"/>
-      <c r="AMI27" s="0"/>
-      <c r="AMJ27" s="0"/>
-    </row>
-    <row r="28" s="56" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="45"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="49"/>
+    </row>
+    <row r="28" s="56" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="52"/>
-      <c r="B28" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" s="57" t="e">
-        <f aca="false">C6+30</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D28" s="58"/>
-      <c r="E28" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="60" t="n">
-        <f aca="false">SUM(G20:G26)</f>
-        <v>2100</v>
-      </c>
+      <c r="B28" s="52"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="55"/>
       <c r="AMF28" s="0"/>
       <c r="AMG28" s="0"/>
       <c r="AMH28" s="0"/>
@@ -1412,12 +1414,13 @@
     <row r="29" s="56" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="52"/>
       <c r="B29" s="52" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="53"/>
+      <c r="C29" s="57" t="e">
+        <f aca="false">C6+30</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D29" s="58"/>
       <c r="E29" s="59" t="s">
         <v>41</v>
       </c>
@@ -1425,8 +1428,8 @@
       <c r="G29" s="59"/>
       <c r="H29" s="59"/>
       <c r="I29" s="60" t="n">
-        <f aca="false">SUM(I20:I26)</f>
-        <v>190</v>
+        <f aca="false">SUM(G21:G27)</f>
+        <v>2100</v>
       </c>
       <c r="AMF29" s="0"/>
       <c r="AMG29" s="0"/>
@@ -1439,19 +1442,19 @@
       <c r="B30" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="62" t="s">
+      <c r="C30" s="61" t="s">
         <v>50</v>
       </c>
       <c r="D30" s="53"/>
       <c r="E30" s="59" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F30" s="59"/>
       <c r="G30" s="59"/>
       <c r="H30" s="59"/>
       <c r="I30" s="60" t="n">
-        <f aca="false">I28+I29</f>
-        <v>2290</v>
+        <f aca="false">SUM(I21:I27)</f>
+        <v>190</v>
       </c>
       <c r="AMF30" s="0"/>
       <c r="AMG30" s="0"/>
@@ -1459,8 +1462,25 @@
       <c r="AMI30" s="0"/>
       <c r="AMJ30" s="0"/>
     </row>
-    <row r="31" s="63" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="64"/>
+    <row r="31" s="56" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="52"/>
+      <c r="B31" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="62" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="53"/>
+      <c r="E31" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="60" t="n">
+        <f aca="false">I29+I30</f>
+        <v>2290</v>
+      </c>
       <c r="AMF31" s="0"/>
       <c r="AMG31" s="0"/>
       <c r="AMH31" s="0"/>
@@ -1468,14 +1488,14 @@
       <c r="AMJ31" s="0"/>
     </row>
     <row r="32" s="63" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="65"/>
+      <c r="C32" s="64"/>
       <c r="AMF32" s="0"/>
       <c r="AMG32" s="0"/>
       <c r="AMH32" s="0"/>
       <c r="AMI32" s="0"/>
       <c r="AMJ32" s="0"/>
     </row>
-    <row r="33" s="63" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" s="63" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="65"/>
       <c r="AMF33" s="0"/>
       <c r="AMG33" s="0"/>
@@ -2203,11 +2223,18 @@
       <c r="AMI123" s="0"/>
       <c r="AMJ123" s="0"/>
     </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="124" s="63" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C124" s="65"/>
+      <c r="AMF124" s="0"/>
+      <c r="AMG124" s="0"/>
+      <c r="AMH124" s="0"/>
+      <c r="AMI124" s="0"/>
+      <c r="AMJ124" s="0"/>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="22">
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="E8:I8"/>
     <mergeCell ref="E9:I9"/>
@@ -2218,7 +2245,7 @@
     <mergeCell ref="F14:I14"/>
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
-    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F17:I17"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
@@ -2226,9 +2253,10 @@
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="E29:H29"/>
     <mergeCell ref="E30:H30"/>
+    <mergeCell ref="E31:H31"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.263194444444444" right="0.236111111111111" top="0.511805555555556" bottom="0.747916666666667" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>